<commit_message>
Refactored Pipeline code, assets, and a level
Day 3
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\dev4\Week_3_Handout\LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B751DB-96F9-4728-97D4-9514EBC95D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B4BDA1-974A-4703-B65F-09A49E1A993E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2030,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,7 +2059,7 @@
         <v>0.02</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LevelMesh structure and level drawing
Day 4
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\dev4\Week_3_Handout\LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B4BDA1-974A-4703-B65F-09A49E1A993E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3843D01-E31E-4B2F-AB37-D214D72CD3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2030,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,7 +2070,7 @@
         <v>0.01</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
         <v>0.03</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Level Renderer parsing Pt 1
Day 5
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\dev4\Week_3_Handout\LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3843D01-E31E-4B2F-AB37-D214D72CD3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9898E499-AE14-495E-BCB4-CA2749D84127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2031,7 +2031,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2081,7 @@
         <v>0.05</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
         <v>0.01</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.08</v>
+        <v>0.13999999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put matrix data in push constant
Weekend
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\dev4\Week_3_Handout\LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9898E499-AE14-495E-BCB4-CA2749D84127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBF64E1-3385-43BA-A86A-2974CFBE6F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2031,7 +2031,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2114,7 @@
         <v>0.1</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.12</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="C50" s="17">
         <f>MIN(SUM(C49,C44,C26,C12),100%)</f>
-        <v>0.13999999999999999</v>
+        <v>0.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better camera, MatrixHelper, and asset updates
Day 7
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\dev4\Week_3_Handout\LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECBC48E2-A84E-414D-9BF1-0005D04571AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191CF1A9-CD16-427D-B876-8920A53A2E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -2031,7 +2031,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>